<commit_message>
Actualiza plantillas de Excel y el historial de clientes. Mejora la lógica de coincidencia de planes en el manejador de plantillas y optimiza la obtención de encabezados de columnas en las hojas de cálculo.
</commit_message>
<xml_diff>
--- a/Bases Consolidados/PANTILLA MANPOWER N.xlsx
+++ b/Bases Consolidados/PANTILLA MANPOWER N.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santi\OneDrive\Escritorio\PROYECTOS\AGENCIA INFONDO\COTIZACIONES\Bases Consolidados Nuevas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santi\OneDrive\Escritorio\PROYECTOS\AGENCIA INFONDO\COTIZACIONES\MCP\Bases Consolidados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31D3BB6B-81B8-461C-929E-06D10210121E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A88533D-61FD-4B2E-BB26-698A4F050A6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{4DEF1856-761C-4FC4-A841-9B5775C87BF6}"/>
+    <workbookView xWindow="-25710" yWindow="10" windowWidth="25820" windowHeight="15500" xr2:uid="{4DEF1856-761C-4FC4-A841-9B5775C87BF6}"/>
   </bookViews>
   <sheets>
     <sheet name="Autos" sheetId="2" r:id="rId1"/>
@@ -255,7 +255,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -496,7 +496,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -516,15 +516,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -555,6 +546,18 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="6" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -594,22 +597,22 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="6" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -928,11 +931,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8971C112-9AF6-42D6-81AB-E2C154B579CA}">
   <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51:E56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.140625" customWidth="1"/>
     <col min="2" max="2" width="33.7109375" customWidth="1"/>
@@ -941,163 +944,163 @@
     <col min="5" max="5" width="31.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="59.1" customHeight="1">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:5" ht="59.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="12" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="13" t="s">
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="12" t="s">
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="13" t="s">
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="12" t="s">
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="12" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="13" t="s">
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="12" t="s">
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="13" t="s">
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="12" t="s">
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="12" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="13" t="s">
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="12" t="s">
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="13" t="s">
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="38" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="22" t="s">
         <v>12</v>
       </c>
       <c r="B19" s="7" t="s">
@@ -1113,8 +1116,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="38"/>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="22"/>
       <c r="B20" s="5" t="s">
         <v>25</v>
       </c>
@@ -1124,600 +1127,600 @@
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="35">
+      <c r="B21" s="19">
         <v>4000000000</v>
       </c>
-      <c r="C21" s="35">
+      <c r="C21" s="19">
         <v>4000000000</v>
       </c>
-      <c r="D21" s="15">
+      <c r="D21" s="12">
         <v>1500000000</v>
       </c>
-      <c r="E21" s="35">
+      <c r="E21" s="19">
         <v>4000000000</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="36"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="15">
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="12">
         <v>1500000000</v>
       </c>
-      <c r="E22" s="36"/>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="E22" s="20"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="37"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="15">
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="12">
         <v>3000000000</v>
       </c>
-      <c r="E23" s="37"/>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="E23" s="21"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D24" s="16" t="s">
+      <c r="D24" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="E24" s="16" t="s">
+      <c r="E24" s="13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="C25" s="16" t="s">
+      <c r="C25" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="D25" s="16" t="s">
+      <c r="D25" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="E25" s="16" t="s">
+      <c r="E25" s="13" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="C26" s="16" t="s">
+      <c r="C26" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="D26" s="16" t="s">
+      <c r="D26" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="E26" s="16" t="s">
+      <c r="E26" s="13" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="D27" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="E27" s="16" t="s">
+      <c r="E27" s="13" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="C28" s="16" t="s">
+      <c r="C28" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="D28" s="16" t="s">
+      <c r="D28" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="E28" s="16" t="s">
+      <c r="E28" s="13" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B29" s="16" t="s">
+      <c r="B29" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="C29" s="16" t="s">
+      <c r="C29" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="D29" s="16" t="s">
+      <c r="D29" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="E29" s="16" t="s">
+      <c r="E29" s="13" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C30" s="16" t="s">
+      <c r="C30" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D30" s="16" t="s">
+      <c r="D30" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="E30" s="16" t="s">
+      <c r="E30" s="13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B31" s="18">
+      <c r="B31" s="15">
         <v>1200000</v>
       </c>
-      <c r="C31" s="18">
+      <c r="C31" s="15">
         <v>1200000</v>
       </c>
-      <c r="D31" s="17" t="s">
+      <c r="D31" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="E31" s="16" t="s">
+      <c r="E31" s="13" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="16" t="s">
+      <c r="C32" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="D32" s="16" t="s">
+      <c r="D32" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="E32" s="16" t="s">
+      <c r="E32" s="13" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B33" s="16" t="s">
+      <c r="B33" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="16" t="s">
+      <c r="C33" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="D33" s="16" t="s">
+      <c r="D33" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="E33" s="16" t="s">
+      <c r="E33" s="13" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C34" s="16" t="s">
+      <c r="C34" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D34" s="16" t="s">
+      <c r="D34" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="E34" s="17" t="s">
+      <c r="E34" s="14" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B35" s="18">
+      <c r="B35" s="15">
         <v>50000000</v>
       </c>
-      <c r="C35" s="18">
+      <c r="C35" s="15">
         <v>50000000</v>
       </c>
-      <c r="D35" s="16"/>
-      <c r="E35" s="18">
+      <c r="D35" s="13"/>
+      <c r="E35" s="15">
         <v>30000000</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="16.5" customHeight="1">
+    <row r="36" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B36" s="16" t="s">
+      <c r="B36" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="C36" s="16" t="s">
+      <c r="C36" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="D36" s="16" t="s">
+      <c r="D36" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="E36" s="16" t="s">
+      <c r="E36" s="13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
     </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="23" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="B38" s="24"/>
-      <c r="C38" s="24"/>
-      <c r="D38" s="24"/>
-      <c r="E38" s="25"/>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="B38" s="25"/>
+      <c r="C38" s="25"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="26"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B39" s="17" t="s">
+      <c r="B39" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="C39" s="17" t="s">
+      <c r="C39" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="D39" s="17" t="s">
+      <c r="D39" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E39" s="17" t="s">
+      <c r="E39" s="14" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B40" s="16" t="s">
+      <c r="B40" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="C40" s="16" t="s">
+      <c r="C40" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D40" s="16" t="s">
+      <c r="D40" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="E40" s="16" t="s">
+      <c r="E40" s="13" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B41" s="16" t="s">
+      <c r="B41" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="C41" s="16" t="s">
+      <c r="C41" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D41" s="16" t="s">
+      <c r="D41" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="E41" s="16" t="s">
+      <c r="E41" s="13" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B42" s="16" t="s">
+      <c r="B42" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="C42" s="16" t="s">
+      <c r="C42" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="D42" s="16" t="s">
+      <c r="D42" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="E42" s="16" t="s">
+      <c r="E42" s="13" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B43" s="17" t="s">
+      <c r="B43" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="C43" s="17" t="s">
+      <c r="C43" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D43" s="17" t="s">
+      <c r="D43" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E43" s="17" t="s">
+      <c r="E43" s="14" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B44" s="16" t="s">
+      <c r="B44" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C44" s="16" t="s">
+      <c r="C44" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D44" s="17" t="s">
+      <c r="D44" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E44" s="16" t="s">
+      <c r="E44" s="13" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B45" s="16" t="s">
+      <c r="B45" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="C45" s="16" t="s">
+      <c r="C45" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="D45" s="16" t="s">
+      <c r="D45" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="E45" s="16" t="s">
+      <c r="E45" s="13" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
     </row>
-    <row r="47" spans="1:5" ht="15.75">
-      <c r="A47" s="26" t="s">
+    <row r="47" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="B47" s="27"/>
-      <c r="C47" s="27"/>
-      <c r="D47" s="27"/>
-      <c r="E47" s="28"/>
-    </row>
-    <row r="48" spans="1:5" ht="15.75">
-      <c r="A48" s="14" t="s">
+      <c r="B47" s="28"/>
+      <c r="C47" s="28"/>
+      <c r="D47" s="28"/>
+      <c r="E47" s="29"/>
+    </row>
+    <row r="48" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B48" s="16" t="s">
+      <c r="B48" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="C48" s="16" t="s">
+      <c r="C48" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="D48" s="16" t="s">
+      <c r="D48" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="E48" s="16" t="s">
+      <c r="E48" s="13" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B49" s="16" t="s">
+      <c r="B49" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C49" s="16" t="s">
+      <c r="C49" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D49" s="16" t="s">
+      <c r="D49" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="E49" s="16" t="s">
+      <c r="E49" s="13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
     </row>
-    <row r="51" spans="1:5" ht="15.75">
-      <c r="A51" s="26" t="s">
+    <row r="51" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="B51" s="27"/>
-      <c r="C51" s="27"/>
-      <c r="D51" s="27"/>
-      <c r="E51" s="28"/>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="4" t="s">
+      <c r="B51" s="28"/>
+      <c r="C51" s="28"/>
+      <c r="D51" s="28"/>
+      <c r="E51" s="29"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="B52" s="19"/>
-      <c r="C52" s="19"/>
-      <c r="D52" s="19"/>
-      <c r="E52" s="19"/>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="A53" s="4" t="s">
+      <c r="B52" s="16"/>
+      <c r="C52" s="16"/>
+      <c r="D52" s="16"/>
+      <c r="E52" s="16"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="B53" s="19">
+      <c r="B53" s="16">
         <v>46157</v>
       </c>
-      <c r="C53" s="19">
+      <c r="C53" s="16">
         <v>45974</v>
       </c>
-      <c r="D53" s="19">
+      <c r="D53" s="16">
         <v>46229</v>
       </c>
-      <c r="E53" s="19">
+      <c r="E53" s="16">
         <v>46224</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
-      <c r="A54" s="4" t="s">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="B54" s="20"/>
-      <c r="C54" s="20"/>
-      <c r="D54" s="20"/>
-      <c r="E54" s="20"/>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="A55" s="9" t="s">
+      <c r="B54" s="17"/>
+      <c r="C54" s="17"/>
+      <c r="D54" s="17"/>
+      <c r="E54" s="17"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="B55" s="10"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10"/>
-      <c r="E55" s="10"/>
-    </row>
-    <row r="56" spans="1:5">
-      <c r="A56" s="9" t="s">
+      <c r="B55" s="40"/>
+      <c r="C55" s="40"/>
+      <c r="D55" s="40"/>
+      <c r="E55" s="40"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="B56" s="11"/>
-      <c r="C56" s="11"/>
-      <c r="D56" s="11"/>
-      <c r="E56" s="11"/>
-    </row>
-    <row r="57" spans="1:5">
+      <c r="B56" s="41"/>
+      <c r="C56" s="41"/>
+      <c r="D56" s="41"/>
+      <c r="E56" s="41"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
     </row>
-    <row r="58" spans="1:5">
-      <c r="A58" s="32" t="s">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B58" s="33"/>
-      <c r="C58" s="33"/>
-      <c r="D58" s="33"/>
-      <c r="E58" s="34"/>
-    </row>
-    <row r="59" spans="1:5" ht="54.95" customHeight="1">
-      <c r="A59" s="29" t="s">
+      <c r="B58" s="34"/>
+      <c r="C58" s="34"/>
+      <c r="D58" s="34"/>
+      <c r="E58" s="35"/>
+    </row>
+    <row r="59" spans="1:5" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="B59" s="30"/>
-      <c r="C59" s="30"/>
-      <c r="D59" s="30"/>
-      <c r="E59" s="31"/>
-    </row>
-    <row r="60" spans="1:5">
+      <c r="B59" s="31"/>
+      <c r="C59" s="31"/>
+      <c r="D59" s="31"/>
+      <c r="E59" s="32"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -1726,17 +1729,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="A47:E47"/>
-    <mergeCell ref="A59:E59"/>
-    <mergeCell ref="A58:E58"/>
-    <mergeCell ref="A51:E51"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
@@ -1750,6 +1742,17 @@
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B11:E11"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A47:E47"/>
+    <mergeCell ref="A59:E59"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="A51:E51"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B17:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1766,6 +1769,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A46240E9C16ACF4580208BCDD1584C19" ma:contentTypeVersion="1" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="c123b30116eb1696ed6760edbcdae06c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="cb24288e-bf72-47ae-a461-19b0293297a2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a9259aa4610e07bbb8461321e94cbc80" ns3:_="">
     <xsd:import namespace="cb24288e-bf72-47ae-a461-19b0293297a2"/>
@@ -1891,12 +1900,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98AAA9BD-141C-449E-9A5F-E23FE59D0BF8}">
   <ds:schemaRefs>
@@ -1906,6 +1909,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{059BE399-E90A-4F5C-8B54-187AC91B948A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="cb24288e-bf72-47ae-a461-19b0293297a2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F720539-AD5F-4FC3-9414-E2EE1548D97C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1921,20 +1940,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{059BE399-E90A-4F5C-8B54-187AC91B948A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="cb24288e-bf72-47ae-a461-19b0293297a2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>